<commit_message>
[Item list] Create headaer added. Not tested
</commit_message>
<xml_diff>
--- a/Docs_and_files/Documents/Files_Block_Diagram.xlsx
+++ b/Docs_and_files/Documents/Files_Block_Diagram.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF2AC4C-024E-4E5C-9832-5DA013D6AECB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE39D9F-0082-4ACF-A9BB-ED648ABFC5DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29730" yWindow="2265" windowWidth="20460" windowHeight="12015" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11940" yWindow="3870" windowWidth="16425" windowHeight="10710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Funkcje" sheetId="2" r:id="rId2"/>
+    <sheet name="Arch" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>void LCD_Init_HW(void);</t>
   </si>
@@ -72,6 +73,75 @@
   </si>
   <si>
     <t>void Switch_SPI_Data_Size(uint8_t Data_Size)</t>
+  </si>
+  <si>
+    <t>void SPI_Send_Data_16bit(...)</t>
+  </si>
+  <si>
+    <t>void SPI_Send_Data_8bit(...)</t>
+  </si>
+  <si>
+    <t>void SPI_Send_Command(...)</t>
+  </si>
+  <si>
+    <t>void MX_SPI2_Init(...)</t>
+  </si>
+  <si>
+    <t>void LCD_Init_HW(...)</t>
+  </si>
+  <si>
+    <t>void LCD_DisplayChar(…)</t>
+  </si>
+  <si>
+    <t>void LCD_Features_Selftest(...)</t>
+  </si>
+  <si>
+    <t>void LCD_DisplayNum(...)</t>
+  </si>
+  <si>
+    <t>void LCD_DisplayString (...)</t>
+  </si>
+  <si>
+    <t>void LCD_DrawCircle(...)</t>
+  </si>
+  <si>
+    <t>void LCD_Configure(...)</t>
+  </si>
+  <si>
+    <t>void Set_Address (...)</t>
+  </si>
+  <si>
+    <t>void LCD_Data_Preparation(...)</t>
+  </si>
+  <si>
+    <t>void Fill_display(...)</t>
+  </si>
+  <si>
+    <t>void LCD_Init(...)</t>
+  </si>
+  <si>
+    <t>void Draw_Point(...)</t>
+  </si>
+  <si>
+    <t>void LCD_DrawLine(...)</t>
+  </si>
+  <si>
+    <t>void LCD_DrawRectangle(...)</t>
+  </si>
+  <si>
+    <t>HAL</t>
+  </si>
+  <si>
+    <t>Middleware</t>
+  </si>
+  <si>
+    <t>App prog interface</t>
+  </si>
+  <si>
+    <t>App code</t>
+  </si>
+  <si>
+    <t>void HAL_StatusTypeDef HAL_SPI_Transmit(...)</t>
   </si>
 </sst>
 </file>
@@ -121,11 +191,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2241,8 +2314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,8 +2329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897D4EBB-321E-45E5-A03B-D7C04464815F}">
   <dimension ref="B11:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,7 +2383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -2335,4 +2408,124 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90F33FC-3498-477D-BF65-AABD3B2421E7}">
+  <dimension ref="B3:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>